<commit_message>
fixed the p-value table
</commit_message>
<xml_diff>
--- a/Tables/region_models_pvalue.xlsx
+++ b/Tables/region_models_pvalue.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haleybranch/Documents/climate_lag/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5862E03-E710-554B-BFDE-A7B9C91C5B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33FA885-F9A1-5045-A76A-DDA4CB66B185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16120" yWindow="680" windowWidth="16960" windowHeight="12780" xr2:uid="{79A1E37C-DB47-3B45-B373-13A3C8B963BE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{79A1E37C-DB47-3B45-B373-13A3C8B963BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="25">
   <si>
     <t xml:space="preserve">Trait </t>
   </si>
@@ -107,9 +107,6 @@
   </si>
   <si>
     <t>South</t>
-  </si>
-  <si>
-    <t>&lt; 00.001</t>
   </si>
   <si>
     <t xml:space="preserve">CMDA </t>
@@ -189,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -233,6 +230,13 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -549,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBAF73EA-FFC3-3548-93D8-97DCF37473CC}">
   <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1039,53 +1043,53 @@
       <c r="F33" s="5"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34">
+      <c r="C34" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="20">
         <v>0</v>
       </c>
       <c r="E34" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F34" s="11">
         <v>2.257E-2</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" s="15">
+      <c r="C35" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="21">
         <v>1</v>
       </c>
       <c r="E35" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="20">
         <v>2.0309999999999998E-3</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D36" s="15">
+      <c r="C36" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="21">
         <v>2</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="20">
         <v>2.539E-3</v>
       </c>
     </row>
@@ -1124,87 +1128,87 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B39" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D39" s="15">
+      <c r="B39" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="21">
         <v>0</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="20">
         <v>1.6910000000000001E-2</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B40" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D40" s="15">
+      <c r="B40" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="21">
         <v>1</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="20">
         <v>4.2779999999999997E-3</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B41" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D41" s="15">
+      <c r="B41" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="21">
         <v>2</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="20">
         <v>8.8889999999999993E-3</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B42" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="B42" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="20" t="s">
         <v>15</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="20">
         <v>8.2920000000000008E-3</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B43" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="B43" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="20" t="s">
         <v>14</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="20">
         <v>7.7400000000000004E-3</v>
       </c>
     </row>
@@ -1294,121 +1298,121 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B49" s="13" t="s">
+      <c r="B49" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C49" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D49" s="15">
+      <c r="C49" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" s="21">
         <v>1</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="20">
         <v>5.3560000000000001E-4</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B50" s="13" t="s">
+      <c r="B50" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C50" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D50" s="15">
+      <c r="C50" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" s="21">
         <v>2</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="20">
         <v>1.0169999999999999E-3</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B51" s="13" t="s">
+      <c r="B51" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C51" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D51" t="s">
+      <c r="C51" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="20" t="s">
         <v>14</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="20">
         <v>5.9949999999999999E-4</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B52" s="13" t="s">
+      <c r="B52" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C52" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D52">
+      <c r="C52" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" s="20">
         <v>0</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="20">
         <v>2.002E-2</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B53" s="13" t="s">
+      <c r="B53" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C53" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D53">
+      <c r="C53" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" s="20">
         <v>2</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F53">
+      <c r="F53" s="20">
         <v>3.125E-2</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B54" s="13" t="s">
+      <c r="B54" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C54" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="C54" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" s="20" t="s">
         <v>15</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F54">
+      <c r="F54" s="20">
         <v>1.8720000000000001E-2</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B55" s="13" t="s">
+      <c r="B55" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C55" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="C55" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" s="20" t="s">
         <v>14</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F55">
+      <c r="F55" s="20">
         <v>1.9650000000000001E-2</v>
       </c>
     </row>
@@ -1623,7 +1627,7 @@
         <v>8</v>
       </c>
       <c r="F68" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.2">
@@ -1696,7 +1700,7 @@
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B73" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C73" s="13" t="s">
         <v>7</v>

</xml_diff>